<commit_message>
adding new non-residential buildings
</commit_message>
<xml_diff>
--- a/data/SIA2024.xlsx
+++ b/data/SIA2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\Test\districtgenerator\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB5F5DD-6E05-40A4-8EF4-46C640F17E2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3459C8C-CD8E-4A51-948C-F569A04F628D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7188" yWindow="12852" windowWidth="23256" windowHeight="12456" tabRatio="799" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="799" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SIA2024" sheetId="13" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="208">
   <si>
     <t>°C</t>
   </si>
@@ -611,9 +611,6 @@
     <t>School</t>
   </si>
   <si>
-    <t>Sale</t>
-  </si>
-  <si>
     <t>Restaurant (with kitchen)</t>
   </si>
   <si>
@@ -654,6 +651,12 @@
   </si>
   <si>
     <t>OB</t>
+  </si>
+  <si>
+    <t>Grocery_store</t>
+  </si>
+  <si>
+    <t>_store</t>
   </si>
 </sst>
 </file>
@@ -761,7 +764,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -776,6 +779,12 @@
     </fill>
     <fill>
       <patternFill patternType="darkTrellis"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="30">
@@ -1205,7 +1214,7 @@
       <protection hidden="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -1271,6 +1280,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="22">
     <cellStyle name="5x indented GHG Textfiels" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1427,10 +1437,10 @@
                   <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.4</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.6</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1</c:v>
@@ -2489,13 +2499,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:CT48"/>
+  <dimension ref="A1:CU48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="BP3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q24" sqref="Q24"/>
+      <selection pane="bottomRight" activeCell="BX8" sqref="BX8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2519,17 +2529,17 @@
     <col min="19" max="19" width="11.140625" customWidth="1"/>
     <col min="86" max="86" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="87" max="87" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="88" max="90" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="22" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="9" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="88" max="91" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="22" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="9" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:98" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:99" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23"/>
       <c r="B1" s="27"/>
       <c r="C1" s="23" t="s">
@@ -2539,7 +2549,7 @@
         <v>0</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F1" s="26" t="s">
         <v>1</v>
@@ -2653,7 +2663,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:98" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:99" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="44" t="s">
         <v>65</v>
       </c>
@@ -2667,7 +2677,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>12</v>
@@ -2916,37 +2926,40 @@
         <v>190</v>
       </c>
       <c r="CJ2" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="CK2" s="4" t="s">
         <v>191</v>
       </c>
       <c r="CL2" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="CM2" s="59" t="s">
+        <v>207</v>
+      </c>
+      <c r="CN2" s="4" t="s">
         <v>192</v>
-      </c>
-      <c r="CM2" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="CN2" s="4" t="s">
-        <v>195</v>
       </c>
       <c r="CO2" s="4" t="s">
         <v>194</v>
       </c>
       <c r="CP2" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="CQ2" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="CR2" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="CQ2" s="4" t="s">
+      <c r="CS2" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="CR2" s="4" t="s">
+      <c r="CT2" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="CS2" s="4" t="s">
-        <v>199</v>
-      </c>
     </row>
-    <row r="3" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>144</v>
       </c>
@@ -3217,19 +3230,22 @@
       <c r="CL3" s="57">
         <v>0</v>
       </c>
-      <c r="CM3" s="57"/>
+      <c r="CM3" s="57">
+        <v>0</v>
+      </c>
       <c r="CN3" s="57"/>
       <c r="CO3" s="57"/>
       <c r="CP3" s="57"/>
       <c r="CQ3" s="57"/>
       <c r="CR3" s="57"/>
       <c r="CS3" s="57"/>
-      <c r="CT3">
-        <f>CJ3*Q3+CJ3*S3</f>
+      <c r="CT3" s="57"/>
+      <c r="CU3">
+        <f t="shared" ref="CU3:CU47" si="0">CJ3*Q3+CJ3*S3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>145</v>
       </c>
@@ -3500,19 +3516,22 @@
       <c r="CL4" s="57">
         <v>0</v>
       </c>
-      <c r="CM4" s="57"/>
+      <c r="CM4" s="57">
+        <v>0</v>
+      </c>
       <c r="CN4" s="57"/>
       <c r="CO4" s="57"/>
       <c r="CP4" s="57"/>
       <c r="CQ4" s="57"/>
       <c r="CR4" s="57"/>
       <c r="CS4" s="57"/>
-      <c r="CT4">
-        <f t="shared" ref="CT4:CT47" si="0">CJ4*Q4+CJ4*S4</f>
+      <c r="CT4" s="57"/>
+      <c r="CU4">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>146</v>
       </c>
@@ -3783,19 +3802,22 @@
       <c r="CL5" s="57">
         <v>0</v>
       </c>
-      <c r="CM5" s="57"/>
+      <c r="CM5" s="57">
+        <v>0</v>
+      </c>
       <c r="CN5" s="57"/>
       <c r="CO5" s="57"/>
       <c r="CP5" s="57"/>
       <c r="CQ5" s="57"/>
       <c r="CR5" s="57"/>
       <c r="CS5" s="57"/>
-      <c r="CT5">
+      <c r="CT5" s="57"/>
+      <c r="CU5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>147</v>
       </c>
@@ -4066,24 +4088,27 @@
       <c r="CL6" s="57">
         <v>0</v>
       </c>
-      <c r="CM6" s="57"/>
+      <c r="CM6" s="57">
+        <v>0</v>
+      </c>
       <c r="CN6" s="57"/>
       <c r="CO6" s="57"/>
       <c r="CP6" s="57"/>
       <c r="CQ6" s="57"/>
       <c r="CR6" s="57"/>
       <c r="CS6" s="57"/>
-      <c r="CT6">
+      <c r="CT6" s="57"/>
+      <c r="CU6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>148</v>
       </c>
       <c r="B7" s="48" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C7" s="1">
         <v>26</v>
@@ -4263,10 +4288,10 @@
         <v>0.8</v>
       </c>
       <c r="BJ7" s="3">
-        <v>0.4</v>
+        <v>0.65</v>
       </c>
       <c r="BK7" s="3">
-        <v>0.6</v>
+        <v>0.65</v>
       </c>
       <c r="BL7" s="3">
         <v>1</v>
@@ -4299,40 +4324,40 @@
         <v>0.1</v>
       </c>
       <c r="BV7" s="16">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="BW7" s="7">
         <v>0.8</v>
       </c>
       <c r="BX7" s="7">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="BY7" s="7">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="BZ7" s="7">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="CA7" s="7">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="CB7" s="7">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="CC7" s="7">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="CD7" s="7">
         <v>0.8</v>
       </c>
       <c r="CE7" s="7">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="CF7" s="7">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="CG7" s="8">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="CH7" s="57">
         <v>0</v>
@@ -4364,16 +4389,19 @@
       <c r="CQ7" s="57">
         <v>0.05</v>
       </c>
-      <c r="CR7" s="57"/>
-      <c r="CS7" s="57">
+      <c r="CR7" s="57">
         <v>0.05</v>
       </c>
-      <c r="CT7">
+      <c r="CS7" s="57"/>
+      <c r="CT7" s="57">
+        <v>0.05</v>
+      </c>
+      <c r="CU7">
         <f t="shared" si="0"/>
         <v>1.73</v>
       </c>
     </row>
-    <row r="8" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>149</v>
       </c>
@@ -4558,10 +4586,10 @@
         <v>0.8</v>
       </c>
       <c r="BJ8" s="3">
-        <v>0.4</v>
+        <v>0.65</v>
       </c>
       <c r="BK8" s="3">
-        <v>0.6</v>
+        <v>0.65</v>
       </c>
       <c r="BL8" s="3">
         <v>1</v>
@@ -4594,40 +4622,40 @@
         <v>0.1</v>
       </c>
       <c r="BV8" s="16">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="BW8" s="7">
         <v>0.8</v>
       </c>
       <c r="BX8" s="7">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="BY8" s="7">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="BZ8" s="7">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="CA8" s="7">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="CB8" s="7">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="CC8" s="7">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="CD8" s="7">
         <v>0.8</v>
       </c>
       <c r="CE8" s="7">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="CF8" s="7">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="CG8" s="8">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="CH8" s="57">
         <v>0</v>
@@ -4644,19 +4672,22 @@
       <c r="CL8" s="57">
         <v>0</v>
       </c>
-      <c r="CM8" s="57"/>
+      <c r="CM8" s="57">
+        <v>0</v>
+      </c>
       <c r="CN8" s="57"/>
       <c r="CO8" s="57"/>
       <c r="CP8" s="57"/>
       <c r="CQ8" s="57"/>
       <c r="CR8" s="57"/>
       <c r="CS8" s="57"/>
-      <c r="CT8">
+      <c r="CT8" s="57"/>
+      <c r="CU8">
         <f t="shared" si="0"/>
         <v>12.3</v>
       </c>
     </row>
-    <row r="9" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>150</v>
       </c>
@@ -4877,40 +4908,40 @@
         <v>0.1</v>
       </c>
       <c r="BV9" s="16">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="BW9" s="7">
         <v>0.8</v>
       </c>
       <c r="BX9" s="7">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="BY9" s="7">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="BZ9" s="7">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="CA9" s="7">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="CB9" s="7">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="CC9" s="7">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="CD9" s="7">
         <v>0.8</v>
       </c>
       <c r="CE9" s="7">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="CF9" s="7">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="CG9" s="8">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="CH9" s="57">
         <v>0</v>
@@ -4927,19 +4958,22 @@
       <c r="CL9" s="57">
         <v>0</v>
       </c>
-      <c r="CM9" s="57"/>
+      <c r="CM9" s="57">
+        <v>0</v>
+      </c>
       <c r="CN9" s="57"/>
       <c r="CO9" s="57"/>
       <c r="CP9" s="57"/>
       <c r="CQ9" s="57"/>
       <c r="CR9" s="57"/>
       <c r="CS9" s="57"/>
-      <c r="CT9">
+      <c r="CT9" s="57"/>
+      <c r="CU9">
         <f t="shared" si="0"/>
         <v>0.8899999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>151</v>
       </c>
@@ -5124,10 +5158,10 @@
         <v>0.8</v>
       </c>
       <c r="BJ10" s="3">
-        <v>0.4</v>
+        <v>0.65</v>
       </c>
       <c r="BK10" s="3">
-        <v>0.6</v>
+        <v>0.65</v>
       </c>
       <c r="BL10" s="3">
         <v>1</v>
@@ -5160,40 +5194,40 @@
         <v>0.1</v>
       </c>
       <c r="BV10" s="16">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="BW10" s="7">
         <v>0.8</v>
       </c>
       <c r="BX10" s="7">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="BY10" s="7">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="BZ10" s="7">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="CA10" s="7">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="CB10" s="7">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="CC10" s="7">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="CD10" s="7">
         <v>0.8</v>
       </c>
       <c r="CE10" s="7">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="CF10" s="7">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="CG10" s="8">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="CH10" s="57">
         <v>0</v>
@@ -5210,19 +5244,22 @@
       <c r="CL10" s="57">
         <v>0</v>
       </c>
-      <c r="CM10" s="57"/>
+      <c r="CM10" s="57">
+        <v>0</v>
+      </c>
       <c r="CN10" s="57"/>
       <c r="CO10" s="57"/>
       <c r="CP10" s="57"/>
       <c r="CQ10" s="57"/>
       <c r="CR10" s="57"/>
       <c r="CS10" s="57"/>
-      <c r="CT10">
+      <c r="CT10" s="57"/>
+      <c r="CU10">
         <f t="shared" si="0"/>
         <v>0.57000000000000006</v>
       </c>
     </row>
-    <row r="11" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>152</v>
       </c>
@@ -5493,19 +5530,22 @@
       <c r="CL11" s="57">
         <v>0</v>
       </c>
-      <c r="CM11" s="57"/>
+      <c r="CM11" s="57">
+        <v>0</v>
+      </c>
       <c r="CN11" s="57"/>
       <c r="CO11" s="57"/>
       <c r="CP11" s="57"/>
       <c r="CQ11" s="57"/>
       <c r="CR11" s="57"/>
       <c r="CS11" s="57"/>
-      <c r="CT11">
+      <c r="CT11" s="57"/>
+      <c r="CU11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>153</v>
       </c>
@@ -5776,19 +5816,22 @@
       <c r="CL12" s="57">
         <v>0</v>
       </c>
-      <c r="CM12" s="57"/>
+      <c r="CM12" s="57">
+        <v>0</v>
+      </c>
       <c r="CN12" s="57"/>
       <c r="CO12" s="57"/>
       <c r="CP12" s="57"/>
       <c r="CQ12" s="57"/>
       <c r="CR12" s="57"/>
       <c r="CS12" s="57"/>
-      <c r="CT12">
+      <c r="CT12" s="57"/>
+      <c r="CU12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>154</v>
       </c>
@@ -6059,19 +6102,22 @@
       <c r="CL13" s="57">
         <v>0</v>
       </c>
-      <c r="CM13" s="57"/>
+      <c r="CM13" s="57">
+        <v>0</v>
+      </c>
       <c r="CN13" s="57"/>
       <c r="CO13" s="57"/>
       <c r="CP13" s="57"/>
       <c r="CQ13" s="57"/>
       <c r="CR13" s="57"/>
       <c r="CS13" s="57"/>
-      <c r="CT13">
+      <c r="CT13" s="57"/>
+      <c r="CU13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>155</v>
       </c>
@@ -6342,19 +6388,22 @@
       <c r="CL14" s="57">
         <v>0</v>
       </c>
-      <c r="CM14" s="57"/>
+      <c r="CM14" s="57">
+        <v>0</v>
+      </c>
       <c r="CN14" s="57"/>
       <c r="CO14" s="57"/>
       <c r="CP14" s="57"/>
       <c r="CQ14" s="57"/>
       <c r="CR14" s="57"/>
       <c r="CS14" s="57"/>
-      <c r="CT14">
+      <c r="CT14" s="57"/>
+      <c r="CU14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>156</v>
       </c>
@@ -6625,19 +6674,22 @@
       <c r="CL15" s="57">
         <v>0</v>
       </c>
-      <c r="CM15" s="57"/>
+      <c r="CM15" s="57">
+        <v>0</v>
+      </c>
       <c r="CN15" s="57"/>
       <c r="CO15" s="57"/>
       <c r="CP15" s="57"/>
       <c r="CQ15" s="57"/>
       <c r="CR15" s="57"/>
       <c r="CS15" s="57"/>
-      <c r="CT15">
+      <c r="CT15" s="57"/>
+      <c r="CU15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>157</v>
       </c>
@@ -6906,26 +6958,30 @@
         <v>0</v>
       </c>
       <c r="CL16" s="57">
-        <v>0.2</v>
-      </c>
-      <c r="CM16" s="57"/>
+        <f>1-SUM(CL3:CL15)-SUM(CL19:CL47)</f>
+        <v>0.59999999999999987</v>
+      </c>
+      <c r="CM16" s="57">
+        <v>0.2</v>
+      </c>
       <c r="CN16" s="57"/>
       <c r="CO16" s="57"/>
       <c r="CP16" s="57"/>
       <c r="CQ16" s="57"/>
       <c r="CR16" s="57"/>
       <c r="CS16" s="57"/>
-      <c r="CT16">
+      <c r="CT16" s="57"/>
+      <c r="CU16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>158</v>
       </c>
       <c r="B17" s="48" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C17" s="1">
         <v>26</v>
@@ -7189,21 +7245,24 @@
         <v>0</v>
       </c>
       <c r="CL17" s="57">
-        <v>0.2</v>
-      </c>
-      <c r="CM17" s="57"/>
+        <v>0</v>
+      </c>
+      <c r="CM17" s="57">
+        <v>0.2</v>
+      </c>
       <c r="CN17" s="57"/>
       <c r="CO17" s="57"/>
       <c r="CP17" s="57"/>
       <c r="CQ17" s="57"/>
       <c r="CR17" s="57"/>
       <c r="CS17" s="57"/>
-      <c r="CT17">
+      <c r="CT17" s="57"/>
+      <c r="CU17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>159</v>
       </c>
@@ -7472,21 +7531,24 @@
         <v>0</v>
       </c>
       <c r="CL18" s="57">
-        <v>0.2</v>
-      </c>
-      <c r="CM18" s="57"/>
+        <v>0</v>
+      </c>
+      <c r="CM18" s="57">
+        <v>0.2</v>
+      </c>
       <c r="CN18" s="57"/>
       <c r="CO18" s="57"/>
       <c r="CP18" s="57"/>
       <c r="CQ18" s="57"/>
       <c r="CR18" s="57"/>
       <c r="CS18" s="57"/>
-      <c r="CT18">
+      <c r="CT18" s="57"/>
+      <c r="CU18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>160</v>
       </c>
@@ -7758,20 +7820,23 @@
         <v>0</v>
       </c>
       <c r="CM19" s="57">
-        <v>0.6</v>
-      </c>
-      <c r="CN19" s="57"/>
+        <v>0</v>
+      </c>
+      <c r="CN19" s="57">
+        <v>0.6</v>
+      </c>
       <c r="CO19" s="57"/>
       <c r="CP19" s="57"/>
       <c r="CQ19" s="57"/>
       <c r="CR19" s="57"/>
       <c r="CS19" s="57"/>
-      <c r="CT19">
+      <c r="CT19" s="57"/>
+      <c r="CU19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>161</v>
       </c>
@@ -8042,19 +8107,22 @@
       <c r="CL20" s="57">
         <v>0</v>
       </c>
-      <c r="CM20" s="57"/>
+      <c r="CM20" s="57">
+        <v>0</v>
+      </c>
       <c r="CN20" s="57"/>
       <c r="CO20" s="57"/>
       <c r="CP20" s="57"/>
       <c r="CQ20" s="57"/>
       <c r="CR20" s="57"/>
       <c r="CS20" s="57"/>
-      <c r="CT20">
+      <c r="CT20" s="57"/>
+      <c r="CU20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>162</v>
       </c>
@@ -8326,20 +8394,23 @@
         <v>0</v>
       </c>
       <c r="CM21" s="57">
-        <v>0.1</v>
-      </c>
-      <c r="CN21" s="57"/>
+        <v>0</v>
+      </c>
+      <c r="CN21" s="57">
+        <v>0.1</v>
+      </c>
       <c r="CO21" s="57"/>
       <c r="CP21" s="57"/>
       <c r="CQ21" s="57"/>
       <c r="CR21" s="57"/>
       <c r="CS21" s="57"/>
-      <c r="CT21">
+      <c r="CT21" s="57"/>
+      <c r="CU21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>163</v>
       </c>
@@ -8610,19 +8681,22 @@
       <c r="CL22" s="57">
         <v>0</v>
       </c>
-      <c r="CM22" s="57"/>
+      <c r="CM22" s="57">
+        <v>0</v>
+      </c>
       <c r="CN22" s="57"/>
       <c r="CO22" s="57"/>
       <c r="CP22" s="57"/>
       <c r="CQ22" s="57"/>
       <c r="CR22" s="57"/>
       <c r="CS22" s="57"/>
-      <c r="CT22">
+      <c r="CT22" s="57"/>
+      <c r="CU22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>164</v>
       </c>
@@ -8893,21 +8967,24 @@
       <c r="CL23" s="57">
         <v>0</v>
       </c>
-      <c r="CM23" s="57"/>
-      <c r="CN23" s="57">
-        <v>0.2</v>
-      </c>
-      <c r="CO23" s="57"/>
+      <c r="CM23" s="57">
+        <v>0</v>
+      </c>
+      <c r="CN23" s="57"/>
+      <c r="CO23" s="57">
+        <v>0.2</v>
+      </c>
       <c r="CP23" s="57"/>
       <c r="CQ23" s="57"/>
       <c r="CR23" s="57"/>
       <c r="CS23" s="57"/>
-      <c r="CT23">
+      <c r="CT23" s="57"/>
+      <c r="CU23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>165</v>
       </c>
@@ -9178,21 +9255,24 @@
       <c r="CL24" s="57">
         <v>0</v>
       </c>
-      <c r="CM24" s="57"/>
-      <c r="CN24" s="57">
-        <v>0.2</v>
-      </c>
-      <c r="CO24" s="57"/>
+      <c r="CM24" s="57">
+        <v>0</v>
+      </c>
+      <c r="CN24" s="57"/>
+      <c r="CO24" s="57">
+        <v>0.2</v>
+      </c>
       <c r="CP24" s="57"/>
       <c r="CQ24" s="57"/>
       <c r="CR24" s="57"/>
       <c r="CS24" s="57"/>
-      <c r="CT24">
+      <c r="CT24" s="57"/>
+      <c r="CU24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>166</v>
       </c>
@@ -9463,21 +9543,24 @@
       <c r="CL25" s="57">
         <v>0</v>
       </c>
-      <c r="CM25" s="57"/>
-      <c r="CN25" s="57">
-        <v>0.2</v>
-      </c>
-      <c r="CO25" s="57"/>
+      <c r="CM25" s="57">
+        <v>0</v>
+      </c>
+      <c r="CN25" s="57"/>
+      <c r="CO25" s="57">
+        <v>0.2</v>
+      </c>
       <c r="CP25" s="57"/>
       <c r="CQ25" s="57"/>
       <c r="CR25" s="57"/>
       <c r="CS25" s="57"/>
-      <c r="CT25">
+      <c r="CT25" s="57"/>
+      <c r="CU25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>167</v>
       </c>
@@ -9748,21 +9831,24 @@
       <c r="CL26" s="57">
         <v>0</v>
       </c>
-      <c r="CM26" s="57"/>
+      <c r="CM26" s="57">
+        <v>0</v>
+      </c>
       <c r="CN26" s="57"/>
-      <c r="CO26" s="57">
+      <c r="CO26" s="57"/>
+      <c r="CP26" s="57">
         <v>0.5</v>
       </c>
-      <c r="CP26" s="57"/>
       <c r="CQ26" s="57"/>
       <c r="CR26" s="57"/>
       <c r="CS26" s="57"/>
-      <c r="CT26">
+      <c r="CT26" s="57"/>
+      <c r="CU26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>168</v>
       </c>
@@ -10033,21 +10119,24 @@
       <c r="CL27" s="57">
         <v>0</v>
       </c>
-      <c r="CM27" s="57"/>
+      <c r="CM27" s="57">
+        <v>0</v>
+      </c>
       <c r="CN27" s="57"/>
-      <c r="CO27" s="57">
+      <c r="CO27" s="57"/>
+      <c r="CP27" s="57">
         <v>0.05</v>
       </c>
-      <c r="CP27" s="57"/>
       <c r="CQ27" s="57"/>
       <c r="CR27" s="57"/>
       <c r="CS27" s="57"/>
-      <c r="CT27">
+      <c r="CT27" s="57"/>
+      <c r="CU27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>169</v>
       </c>
@@ -10318,21 +10407,24 @@
       <c r="CL28" s="57">
         <v>0</v>
       </c>
-      <c r="CM28" s="57"/>
+      <c r="CM28" s="57">
+        <v>0</v>
+      </c>
       <c r="CN28" s="57"/>
-      <c r="CO28" s="57">
-        <v>0.1</v>
-      </c>
-      <c r="CP28" s="57"/>
+      <c r="CO28" s="57"/>
+      <c r="CP28" s="57">
+        <v>0.1</v>
+      </c>
       <c r="CQ28" s="57"/>
       <c r="CR28" s="57"/>
       <c r="CS28" s="57"/>
-      <c r="CT28">
+      <c r="CT28" s="57"/>
+      <c r="CU28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>170</v>
       </c>
@@ -10603,21 +10695,24 @@
       <c r="CL29" s="57">
         <v>0</v>
       </c>
-      <c r="CM29" s="57"/>
+      <c r="CM29" s="57">
+        <v>0</v>
+      </c>
       <c r="CN29" s="57"/>
       <c r="CO29" s="57"/>
-      <c r="CP29" s="57">
-        <v>0.1</v>
-      </c>
-      <c r="CQ29" s="57"/>
+      <c r="CP29" s="57"/>
+      <c r="CQ29" s="57">
+        <v>0.1</v>
+      </c>
       <c r="CR29" s="57"/>
       <c r="CS29" s="57"/>
-      <c r="CT29">
+      <c r="CT29" s="57"/>
+      <c r="CU29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>171</v>
       </c>
@@ -10888,21 +10983,24 @@
       <c r="CL30" s="57">
         <v>0</v>
       </c>
-      <c r="CM30" s="57"/>
+      <c r="CM30" s="57">
+        <v>0</v>
+      </c>
       <c r="CN30" s="57"/>
       <c r="CO30" s="57"/>
-      <c r="CP30" s="57">
-        <v>0.6</v>
-      </c>
-      <c r="CQ30" s="57"/>
+      <c r="CP30" s="57"/>
+      <c r="CQ30" s="57">
+        <v>0.6</v>
+      </c>
       <c r="CR30" s="57"/>
       <c r="CS30" s="57"/>
-      <c r="CT30">
+      <c r="CT30" s="57"/>
+      <c r="CU30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>172</v>
       </c>
@@ -11173,19 +11271,22 @@
       <c r="CL31" s="57">
         <v>0</v>
       </c>
-      <c r="CM31" s="57"/>
+      <c r="CM31" s="57">
+        <v>0</v>
+      </c>
       <c r="CN31" s="57"/>
       <c r="CO31" s="57"/>
       <c r="CP31" s="57"/>
       <c r="CQ31" s="57"/>
       <c r="CR31" s="57"/>
       <c r="CS31" s="57"/>
-      <c r="CT31">
+      <c r="CT31" s="57"/>
+      <c r="CU31">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>173</v>
       </c>
@@ -11456,21 +11557,24 @@
       <c r="CL32" s="57">
         <v>0</v>
       </c>
-      <c r="CM32" s="57"/>
+      <c r="CM32" s="57">
+        <v>0</v>
+      </c>
       <c r="CN32" s="57"/>
       <c r="CO32" s="57"/>
       <c r="CP32" s="57"/>
-      <c r="CQ32" s="57">
-        <v>0.8</v>
-      </c>
-      <c r="CR32" s="57"/>
+      <c r="CQ32" s="57"/>
+      <c r="CR32" s="57">
+        <v>0.8</v>
+      </c>
       <c r="CS32" s="57"/>
-      <c r="CT32">
+      <c r="CT32" s="57"/>
+      <c r="CU32">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>174</v>
       </c>
@@ -11741,21 +11845,24 @@
       <c r="CL33" s="57">
         <v>0</v>
       </c>
-      <c r="CM33" s="57"/>
+      <c r="CM33" s="57">
+        <v>0</v>
+      </c>
       <c r="CN33" s="57"/>
       <c r="CO33" s="57"/>
       <c r="CP33" s="57"/>
       <c r="CQ33" s="57"/>
-      <c r="CR33" s="57">
+      <c r="CR33" s="57"/>
+      <c r="CS33" s="57">
         <v>0.7</v>
       </c>
-      <c r="CS33" s="57"/>
-      <c r="CT33">
+      <c r="CT33" s="57"/>
+      <c r="CU33">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>175</v>
       </c>
@@ -12026,19 +12133,22 @@
       <c r="CL34" s="57">
         <v>0</v>
       </c>
-      <c r="CM34" s="57"/>
+      <c r="CM34" s="57">
+        <v>0</v>
+      </c>
       <c r="CN34" s="57"/>
       <c r="CO34" s="57"/>
       <c r="CP34" s="57"/>
       <c r="CQ34" s="57"/>
       <c r="CR34" s="57"/>
       <c r="CS34" s="57"/>
-      <c r="CT34">
+      <c r="CT34" s="57"/>
+      <c r="CU34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>176</v>
       </c>
@@ -12309,26 +12419,29 @@
       <c r="CL35" s="57">
         <v>0</v>
       </c>
-      <c r="CM35" s="57"/>
+      <c r="CM35" s="57">
+        <v>0</v>
+      </c>
       <c r="CN35" s="57"/>
       <c r="CO35" s="57"/>
       <c r="CP35" s="57"/>
       <c r="CQ35" s="57"/>
       <c r="CR35" s="57"/>
-      <c r="CS35" s="57">
-        <v>0.6</v>
-      </c>
-      <c r="CT35">
+      <c r="CS35" s="57"/>
+      <c r="CT35" s="57">
+        <v>0.6</v>
+      </c>
+      <c r="CU35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>177</v>
       </c>
       <c r="B36" s="48" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C36" s="1">
         <v>26</v>
@@ -12598,10 +12711,10 @@
         <v>0.1</v>
       </c>
       <c r="CN36" s="57">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="CO36" s="57">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="CP36" s="57">
         <v>0.05</v>
@@ -12610,17 +12723,20 @@
         <v>0.05</v>
       </c>
       <c r="CR36" s="57">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="CS36" s="57">
         <v>0.1</v>
       </c>
-      <c r="CT36">
+      <c r="CT36" s="57">
+        <v>0.1</v>
+      </c>
+      <c r="CU36">
         <f t="shared" si="0"/>
         <v>0.34</v>
       </c>
     </row>
-    <row r="37" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>178</v>
       </c>
@@ -12891,23 +13007,26 @@
       <c r="CL37" s="57">
         <v>0</v>
       </c>
-      <c r="CM37" s="57"/>
+      <c r="CM37" s="57">
+        <v>0</v>
+      </c>
       <c r="CN37" s="57"/>
-      <c r="CO37" s="57">
-        <v>0.05</v>
-      </c>
+      <c r="CO37" s="57"/>
       <c r="CP37" s="57">
         <v>0.05</v>
       </c>
-      <c r="CQ37" s="57"/>
+      <c r="CQ37" s="57">
+        <v>0.05</v>
+      </c>
       <c r="CR37" s="57"/>
       <c r="CS37" s="57"/>
-      <c r="CT37">
+      <c r="CT37" s="57"/>
+      <c r="CU37">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>179</v>
       </c>
@@ -13178,23 +13297,26 @@
       <c r="CL38" s="57">
         <v>0.05</v>
       </c>
-      <c r="CM38" s="57"/>
+      <c r="CM38" s="57">
+        <v>0.05</v>
+      </c>
       <c r="CN38" s="57"/>
-      <c r="CO38" s="57">
-        <v>0.05</v>
-      </c>
+      <c r="CO38" s="57"/>
       <c r="CP38" s="57">
         <v>0.05</v>
       </c>
-      <c r="CQ38" s="57"/>
+      <c r="CQ38" s="57">
+        <v>0.05</v>
+      </c>
       <c r="CR38" s="57"/>
       <c r="CS38" s="57"/>
-      <c r="CT38">
+      <c r="CT38" s="57"/>
+      <c r="CU38">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>180</v>
       </c>
@@ -13466,7 +13588,7 @@
         <v>0.15</v>
       </c>
       <c r="CM39" s="57">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="CN39" s="57">
         <v>0.1</v>
@@ -13486,17 +13608,20 @@
       <c r="CS39" s="57">
         <v>0.1</v>
       </c>
-      <c r="CT39">
+      <c r="CT39" s="57">
+        <v>0.1</v>
+      </c>
+      <c r="CU39">
         <f t="shared" si="0"/>
         <v>2.0000000000000004E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>181</v>
       </c>
       <c r="B40" s="48" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C40" s="1">
         <v>26</v>
@@ -13712,40 +13837,40 @@
         <v>0.1</v>
       </c>
       <c r="BV40" s="16">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="BW40" s="7">
         <v>0.8</v>
       </c>
       <c r="BX40" s="7">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="BY40" s="7">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="BZ40" s="7">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="CA40" s="7">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="CB40" s="7">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="CC40" s="7">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="CD40" s="7">
         <v>0.8</v>
       </c>
       <c r="CE40" s="7">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="CF40" s="7">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="CG40" s="8">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="CH40" s="57">
         <v>0</v>
@@ -13762,19 +13887,22 @@
       <c r="CL40" s="57">
         <v>0</v>
       </c>
-      <c r="CM40" s="57"/>
+      <c r="CM40" s="57">
+        <v>0</v>
+      </c>
       <c r="CN40" s="57"/>
       <c r="CO40" s="57"/>
       <c r="CP40" s="57"/>
       <c r="CQ40" s="57"/>
       <c r="CR40" s="57"/>
       <c r="CS40" s="57"/>
-      <c r="CT40">
+      <c r="CT40" s="57"/>
+      <c r="CU40">
         <f t="shared" si="0"/>
         <v>1.37</v>
       </c>
     </row>
-    <row r="41" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>182</v>
       </c>
@@ -14045,19 +14173,22 @@
       <c r="CL41" s="57">
         <v>0</v>
       </c>
-      <c r="CM41" s="57"/>
+      <c r="CM41" s="57">
+        <v>0</v>
+      </c>
       <c r="CN41" s="57"/>
       <c r="CO41" s="57"/>
       <c r="CP41" s="57"/>
       <c r="CQ41" s="57"/>
       <c r="CR41" s="57"/>
       <c r="CS41" s="57"/>
-      <c r="CT41">
+      <c r="CT41" s="57"/>
+      <c r="CU41">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>183</v>
       </c>
@@ -14328,27 +14459,30 @@
       <c r="CL42" s="57">
         <v>0</v>
       </c>
-      <c r="CM42" s="57"/>
-      <c r="CN42" s="57">
-        <v>0.05</v>
-      </c>
+      <c r="CM42" s="57">
+        <v>0</v>
+      </c>
+      <c r="CN42" s="57"/>
       <c r="CO42" s="57">
         <v>0.05</v>
       </c>
-      <c r="CP42" s="57"/>
+      <c r="CP42" s="57">
+        <v>0.05</v>
+      </c>
       <c r="CQ42" s="57"/>
-      <c r="CR42" s="57">
-        <v>0.05</v>
-      </c>
+      <c r="CR42" s="57"/>
       <c r="CS42" s="57">
         <v>0.05</v>
       </c>
-      <c r="CT42">
+      <c r="CT42" s="57">
+        <v>0.05</v>
+      </c>
+      <c r="CU42">
         <f t="shared" si="0"/>
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>184</v>
       </c>
@@ -14622,22 +14756,25 @@
       <c r="CM43" s="57">
         <v>0.05</v>
       </c>
-      <c r="CN43" s="57"/>
+      <c r="CN43" s="57">
+        <v>0.05</v>
+      </c>
       <c r="CO43" s="57"/>
       <c r="CP43" s="57"/>
       <c r="CQ43" s="57"/>
-      <c r="CR43" s="57">
+      <c r="CR43" s="57"/>
+      <c r="CS43" s="57">
         <v>0.05</v>
       </c>
-      <c r="CS43" s="57">
-        <v>0.1</v>
-      </c>
-      <c r="CT43">
+      <c r="CT43" s="57">
+        <v>0.1</v>
+      </c>
+      <c r="CU43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>185</v>
       </c>
@@ -14908,19 +15045,22 @@
       <c r="CL44" s="57">
         <v>0</v>
       </c>
-      <c r="CM44" s="57"/>
+      <c r="CM44" s="57">
+        <v>0</v>
+      </c>
       <c r="CN44" s="57"/>
       <c r="CO44" s="57"/>
       <c r="CP44" s="57"/>
       <c r="CQ44" s="57"/>
       <c r="CR44" s="57"/>
       <c r="CS44" s="57"/>
-      <c r="CT44">
+      <c r="CT44" s="57"/>
+      <c r="CU44">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>143</v>
       </c>
@@ -15191,19 +15331,22 @@
       <c r="CL45" s="57">
         <v>0</v>
       </c>
-      <c r="CM45" s="57"/>
+      <c r="CM45" s="57">
+        <v>0</v>
+      </c>
       <c r="CN45" s="57"/>
       <c r="CO45" s="57"/>
       <c r="CP45" s="57"/>
       <c r="CQ45" s="57"/>
       <c r="CR45" s="57"/>
       <c r="CS45" s="57"/>
-      <c r="CT45">
+      <c r="CT45" s="57"/>
+      <c r="CU45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>186</v>
       </c>
@@ -15474,19 +15617,22 @@
       <c r="CL46" s="57">
         <v>0</v>
       </c>
-      <c r="CM46" s="57"/>
+      <c r="CM46" s="57">
+        <v>0</v>
+      </c>
       <c r="CN46" s="57"/>
       <c r="CO46" s="57"/>
       <c r="CP46" s="57"/>
       <c r="CQ46" s="57"/>
       <c r="CR46" s="57"/>
       <c r="CS46" s="57"/>
-      <c r="CT46">
+      <c r="CT46" s="57"/>
+      <c r="CU46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:98" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:99" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="10" t="s">
         <v>187</v>
       </c>
@@ -15757,19 +15903,22 @@
       <c r="CL47" s="57">
         <v>0</v>
       </c>
-      <c r="CM47" s="57"/>
+      <c r="CM47" s="57">
+        <v>0</v>
+      </c>
       <c r="CN47" s="57"/>
       <c r="CO47" s="57"/>
       <c r="CP47" s="57"/>
       <c r="CQ47" s="57"/>
       <c r="CR47" s="57"/>
       <c r="CS47" s="57"/>
-      <c r="CT47">
+      <c r="CT47" s="57"/>
+      <c r="CU47">
         <f t="shared" si="0"/>
         <v>7.0519999999999996</v>
       </c>
     </row>
-    <row r="48" spans="1:98" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:99" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="38" t="s">
         <v>66</v>
       </c>
@@ -16030,7 +16179,7 @@
         <v>1</v>
       </c>
       <c r="CJ48" s="58">
-        <f t="shared" ref="CJ48:CS48" si="1">SUM(CJ4:CJ47)</f>
+        <f t="shared" ref="CJ48:CL48" si="1">SUM(CJ4:CJ47)</f>
         <v>1</v>
       </c>
       <c r="CK48" s="58">
@@ -16042,35 +16191,39 @@
         <v>1</v>
       </c>
       <c r="CM48" s="58">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="CM48" si="2">SUM(CM4:CM47)</f>
         <v>1</v>
       </c>
       <c r="CN48" s="58">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="CN48:CT48" si="3">SUM(CN4:CN47)</f>
         <v>1</v>
       </c>
       <c r="CO48" s="58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="CP48" s="58">
+        <f t="shared" si="3"/>
         <v>1.0000000000000002</v>
       </c>
-      <c r="CP48" s="58">
-        <f t="shared" si="1"/>
+      <c r="CQ48" s="58">
+        <f t="shared" si="3"/>
         <v>1.0000000000000002</v>
       </c>
-      <c r="CQ48" s="58">
-        <f t="shared" si="1"/>
+      <c r="CR48" s="58">
+        <f t="shared" si="3"/>
         <v>1.0000000000000002</v>
       </c>
-      <c r="CR48" s="58">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
       <c r="CS48" s="58">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="CT48" s="6">
-        <f>SUM(CT3:CT47)</f>
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="CT48" s="58">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="CU48" s="6">
+        <f>SUM(CU3:CU47)</f>
         <v>24.338000000000001</v>
       </c>
     </row>

</xml_diff>